<commit_message>
removed xlsx file filter
</commit_message>
<xml_diff>
--- a/migration/questions.xlsx
+++ b/migration/questions.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="758" uniqueCount="228">
   <si>
     <t>Index</t>
   </si>
@@ -708,6 +708,9 @@
   </si>
   <si>
     <t>Percentile</t>
+  </si>
+  <si>
+    <t>q</t>
   </si>
 </sst>
 </file>
@@ -1180,7 +1183,7 @@
   <dimension ref="A1:E168"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -2445,7 +2448,7 @@
         <v>18</v>
       </c>
       <c r="E74" t="s">
-        <v>15</v>
+        <v>227</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -4423,7 +4426,7 @@
   <dimension ref="A1:L8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>

</xml_diff>